<commit_message>
Worked on the effects doc. + Cleaned the Samurai skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/8-Samurai/Documentation/SamuraiSkills.xlsx
+++ b/GameDesign/Class/_Done/8-Samurai/Documentation/SamuraiSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Dō-Maru" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>Additional Info</t>
   </si>
@@ -101,15 +101,6 @@
     <t>[[Number of turns between two casts: 2 ]]</t>
   </si>
   <si>
-    <t>[[Damage:  15-20 earth ]]</t>
-  </si>
-  <si>
-    <t>Target: [[Reduce resistance by 25%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage and reduce resistance.</t>
-  </si>
-  <si>
     <t>Bokken</t>
   </si>
   <si>
@@ -122,42 +113,6 @@
     <t>[[Number of cast per turn per target: 3 ]]</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 10 ]]</t>
-  </si>
-  <si>
-    <t>Effect name: ''Bokken''.</t>
-  </si>
-  <si>
-    <t>If the caster is under ''Keikogi'' effect:</t>
-  </si>
-  <si>
-    <t>If the caster is not under ''Keikogi'' effect:</t>
-  </si>
-  <si>
-    <t>When effect reach lvl 10, all the stacked effect are set to 2 turns.</t>
-  </si>
-  <si>
-    <t>[[Area of effect: - Single cell ]] (Must target an entity)</t>
-  </si>
-  <si>
-    <t>Stealth Air-type health                                                                        OR                                                                                                 Inflicts Earth-type damage.                                                                                                                                                                    Increase melee damage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Target: [[Damage: 15-20 earth]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Caster: [[''Bokken'' effect +1 lvl]] (2 turns)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Target: [[Damage:  15-20 air steal ]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Caster: [[''Bokken'' effect +2 lvl]] (2 turns) </t>
-  </si>
-  <si>
-    <t>Caster: [[Boost melee damage by 10%]] (2 turns)</t>
-  </si>
-  <si>
     <t>Hara-Kiri</t>
   </si>
   <si>
@@ -173,18 +128,6 @@
     <t>[[Area of effect: - All the map ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Hara-Kiri''.</t>
-  </si>
-  <si>
-    <t>Enemies: [[Increase taken damage by 25%]] (1 turn)</t>
-  </si>
-  <si>
-    <t>Allies: [[Increase damage by 25%]] (2 turns)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caster: [[Set K/O]] </t>
-  </si>
-  <si>
     <t>The caster die to boost all his allies and weaken all his enemies.   The caster can only do it when his HP are at 20% or less.</t>
   </si>
   <si>
@@ -203,57 +146,18 @@
     <t>[[Cast in straight line: No ]]</t>
   </si>
   <si>
-    <t>[[Damage:  5-50 air ]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Caster: [[''Yumi'' effect +1 lvl]] (2 turns)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Yumi''.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Caster: [[Boost ranged damage by 10%]] (8 turns)</t>
-  </si>
-  <si>
-    <t>Inflicts Air-type damage and Increase ranged damage.</t>
-  </si>
-  <si>
     <t>Kiai</t>
   </si>
   <si>
     <t>[[Area of effect: - Circle of 2 cells radius ]]</t>
   </si>
   <si>
-    <t>Enemies: [[Damage: 5-10 air ]]</t>
-  </si>
-  <si>
-    <t>Caster: [[Increase next skill damage by 30%]]</t>
-  </si>
-  <si>
-    <t>Allies:  [[Increase next skill damage by 20%]]</t>
-  </si>
-  <si>
-    <t>Effect name: ''Kiai''.</t>
-  </si>
-  <si>
-    <t>Inflicts Air-type damage and increase the damage of the next skill.</t>
-  </si>
-  <si>
     <t>Jinsoku</t>
   </si>
   <si>
     <t>[[Number of turns between two casts: 4 ]]</t>
   </si>
   <si>
-    <t>[[Increase MP by MP / 2 (rounded up)]] (1 turn)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Jinsoku''.</t>
-  </si>
-  <si>
-    <t>Increase the caster speed.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Unbuff </t>
     </r>
@@ -446,6 +350,361 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> +1 level (4 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage and reduce resistance.</t>
+  </si>
+  <si>
+    <t>[[Damage:  15-20 ground ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vulnerable]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Stealth Wind-type health                                                                        OR                                                                                                 Inflicts Ground-type damage.                                                                                                                                                                    Increase melee damage.                                                                          Must target an entity.</t>
+  </si>
+  <si>
+    <t>Else:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage:  15-20 wind steal ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 15-20 ground]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If caster have </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Keikogi]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Caster: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Melee]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +20 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Caster: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Melee]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +10 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[[K/O]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allies: </t>
+  </si>
+  <si>
+    <t>Enemies:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Stimulated]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +5 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Melee]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +50 levels (1 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blindness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 10 levels (1 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vitality]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +10 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Speed]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +5 levels (1 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Void]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +30 (2 turns) </t>
+    </r>
+  </si>
+  <si>
+    <t>Inflicts Wind-type damage and Increase ranged damage.</t>
+  </si>
+  <si>
+    <t>[[Damage: 5-50 wind ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Caster: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Ranged]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +10 level (6 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Increase the damage of the next skill of the caster and his allies.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Caster: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Preparation]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +30 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Allies:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Preparation]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 15 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Increase the caster speed by half of his remaining MP.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Speed]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +(MP / 2 (rounded up)) levels (1 turns)</t>
     </r>
   </si>
 </sst>
@@ -518,7 +777,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -587,11 +846,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -616,7 +895,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -632,6 +910,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,7 +1261,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1055,14 +1335,14 @@
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="9" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1109,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1130,7 +1410,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1142,7 +1422,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1154,7 +1434,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -1185,7 +1465,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1209,7 +1489,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1238,9 +1518,7 @@
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="C22" s="7"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -1291,7 +1569,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1365,14 +1643,14 @@
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="9" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1525,36 +1803,36 @@
     </row>
     <row r="17" spans="2:4" ht="78" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="18" t="s">
-        <v>79</v>
+      <c r="C17" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="17" t="s">
-        <v>83</v>
+      <c r="C18" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="19" t="s">
-        <v>82</v>
+      <c r="C19" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="14" t="s">
-        <v>80</v>
+      <c r="C20" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="15" t="s">
-        <v>81</v>
+      <c r="C21" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1602,7 +1880,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,7 +1912,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1708,14 +1986,14 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="11" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="15" t="s">
-        <v>86</v>
+      <c r="C18" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1762,7 +2040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1795,7 +2073,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1862,14 +2140,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1914,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +2215,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1946,10 +2224,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>35</v>
+      <c r="C5" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1961,167 +2239,146 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="C15" s="7"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="11" t="s">
-        <v>31</v>
+      <c r="C19" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="14" t="s">
-        <v>38</v>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="12" t="s">
-        <v>39</v>
+      <c r="C21" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="11" t="s">
-        <v>32</v>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="14" t="s">
-        <v>36</v>
+      <c r="C23" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
+    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="1"/>
+      <c r="C27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="1"/>
-      <c r="C32" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="16"/>
+      <c r="D30" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2131,10 +2388,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,7 +2411,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2166,7 +2423,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2178,14 +2435,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2216,7 +2473,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2228,7 +2485,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2240,58 +2497,105 @@
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="9" t="s">
-        <v>48</v>
+      <c r="C18" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="9" t="s">
-        <v>47</v>
+      <c r="C19" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="4" t="s">
-        <v>0</v>
+      <c r="C23" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="7" t="s">
-        <v>46</v>
+      <c r="C25" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="5"/>
+      <c r="C26" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B30" s="1"/>
+      <c r="C30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2301,10 +2605,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2628,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2336,7 +2640,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2362,7 +2666,7 @@
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2374,21 +2678,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2400,108 +2704,87 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
+      <c r="C20" s="20" t="s">
+        <v>75</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="2" t="s">
-        <v>56</v>
+      <c r="C22" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2511,10 +2794,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2534,7 +2817,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2543,10 +2826,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2601,7 +2884,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2613,58 +2896,49 @@
     <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="9" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>